<commit_message>
final universal table create for leather project
</commit_message>
<xml_diff>
--- a/JBC_office_work/Leather/ETL/universal_table.xlsx
+++ b/JBC_office_work/Leather/ETL/universal_table.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>internal_memo</t>
   </si>
@@ -22,13 +25,7 @@
     <t>customer_memo</t>
   </si>
   <si>
-    <t>order_id_or_management_number</t>
-  </si>
-  <si>
-    <t>expert_description</t>
-  </si>
-  <si>
-    <t>order_items_id</t>
+    <t>description</t>
   </si>
   <si>
     <t>description_template_id</t>
@@ -722,24 +719,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>44206</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2">
-        <v>44206</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2">
         <v>46909</v>
@@ -749,17 +746,17 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>44206</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>44206</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>46944</v>
@@ -769,17 +766,17 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>44206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>44206</v>
-      </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>46910</v>
@@ -789,17 +786,17 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>44206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>44206</v>
-      </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>46910</v>

</xml_diff>